<commit_message>
plot(ISGT): moved Time x-axis text to right
</commit_message>
<xml_diff>
--- a/main/results/ISGT/ISGT_summary.xlsx
+++ b/main/results/ISGT/ISGT_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergi Costa\Documents\agistin\main\results\ISGT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BDE170-A4ED-42EE-A353-8CB1AD1B7975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D451A5-16CD-44AF-97A8-C51282837513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24615" yWindow="480" windowWidth="16305" windowHeight="9015" xr2:uid="{BD5D70AB-A72A-407F-9497-CDFDE3A85D19}"/>
+    <workbookView xWindow="-27525" yWindow="1710" windowWidth="16305" windowHeight="9015" xr2:uid="{BD5D70AB-A72A-407F-9497-CDFDE3A85D19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,6 +64,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -99,9 +102,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,7 +424,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,19 +481,19 @@
       <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="3">
         <f>B2/60</f>
         <v>8.4691198031107504</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="3">
         <f>C2/60</f>
         <v>11.318881706396732</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="3">
         <f>D2/60</f>
         <v>65.840855002403174</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="3">
         <f>E2/60</f>
         <v>6.6739318370818994</v>
       </c>
@@ -513,19 +518,19 @@
       <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="2">
         <f>B3/2</f>
         <v>12.481616647320401</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="2">
         <f>C3/2</f>
         <v>6.4524089560012996</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="2">
         <f>D3/2</f>
         <v>-14.755192021108099</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="2">
         <f>E3/2</f>
         <v>-15.114467563663201</v>
       </c>

</xml_diff>

<commit_message>
style: reformatted and cleaned ISGT results summary
</commit_message>
<xml_diff>
--- a/main/results/ISGT/ISGT_summary.xlsx
+++ b/main/results/ISGT/ISGT_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergi Costa\Documents\agistin\main\results\ISGT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D451A5-16CD-44AF-97A8-C51282837513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53731A90-F712-4002-A95C-17A48D5EA625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27525" yWindow="1710" windowWidth="16305" windowHeight="9015" xr2:uid="{BD5D70AB-A72A-407F-9497-CDFDE3A85D19}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BD5D70AB-A72A-407F-9497-CDFDE3A85D19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -106,7 +106,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,7 +424,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,6 +535,20 @@
         <v>-15.114467563663201</v>
       </c>
     </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <f>I3/$H$3</f>
+        <v>0.51695298280023094</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:K4" si="0">J3/$H$3</f>
+        <v>-1.1821539178801648</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>-1.2109382935509425</v>
+      </c>
+    </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>

</xml_diff>